<commit_message>
Merged new data file from dev to master
</commit_message>
<xml_diff>
--- a/data/data_US9410_02.xlsx
+++ b/data/data_US9410_02.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>oppID</t>
   </si>
@@ -25,6 +25,9 @@
     <t>thirdParty</t>
   </si>
   <si>
+    <t>726722-B21</t>
+  </si>
+  <si>
     <t>G1S72A</t>
   </si>
   <si>
@@ -55,7 +58,16 @@
     <t>OPE-0002935252</t>
   </si>
   <si>
-    <t>ZU706A</t>
+    <t>user</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>apassword</t>
   </si>
 </sst>
 </file>
@@ -404,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +432,7 @@
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,39 +443,51 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging dev into master
</commit_message>
<xml_diff>
--- a/data/data_US9410_02.xlsx
+++ b/data/data_US9410_02.xlsx
@@ -64,17 +64,17 @@
     <t>pass</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>apassword</t>
+    <t>taousautotester@hpe.com</t>
+  </si>
+  <si>
+    <t>5810ca086fd249fe54f03436d5829007179d176ceef6d120c899</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +84,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,14 +114,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,7 +430,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +494,7 @@
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -491,7 +502,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="mailto:taousautotester@hpe.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>